<commit_message>
[add] ptn de bloc
</commit_message>
<xml_diff>
--- a/result/guigui2- FR001400B4A4.xlsx
+++ b/result/guigui2- FR001400B4A4.xlsx
@@ -558,7 +558,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>coupon autocall</t>
+          <t>coupon phoenix</t>
         </is>
       </c>
     </row>
@@ -575,7 +575,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>trimestre</t>
+          <t>année</t>
         </is>
       </c>
     </row>
@@ -592,7 +592,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>12</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bouygues SA</t>
+          <t>Bouygues SA et BNP Paribas</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>mono action</t>
+          <t>wo action</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>degressif</t>
         </is>
       </c>
     </row>
@@ -677,7 +677,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>81</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>80</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>80</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>29/07/2030</t>
+          <t>29/07/2026</t>
         </is>
       </c>
     </row>
@@ -864,7 +864,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>29/07/2032</t>
+          <t>29/07/2027</t>
         </is>
       </c>
     </row>
@@ -915,7 +915,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>02/08/2030</t>
+          <t>02/08/2026</t>
         </is>
       </c>
     </row>
@@ -932,7 +932,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>02/08/2032</t>
+          <t>02/08/2027</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1065,7 +1065,35 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-12.21</t>
+          <t>-22.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1080,7 +1108,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
@@ -1098,21 +1126,35 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>31/07/2023, 30/10/2023, 29/01/2024, 29/04/2024, 29/07/2024, 29/10/2024, 29/01/2025, 29/04/2025, 29/07/2025, 29/10/2025, 29/01/2026, 29/04/2026, 29/07/2026, 29/10/2026, 29/01/2027, 29/04/2027, 29/07/2027, 29/10/2027, 31/01/2028, 02/05/2028, 31/07/2028, 30/10/2028, 29/01/2029, 30/04/2029, 30/07/2029, 29/10/2029, 29/01/2030, 29/04/2030, 29/07/2030, 29/10/2030, 29/01/2031, 29/04/2031, 29/07/2031, 29/10/2031, 29/01/2032, 29/04/2032, 29/07/2032, 29/07/2032</t>
+          <t>31/07/2023, 29/07/2024, 29/07/2025, 29/07/2026, 29/07/2027, 29/07/2027</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dates de remboursement</t>
+          <t>Dates de paiement1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>07/08/2023, 06/11/2023, 05/02/2024, 07/05/2024, 05/08/2024, 05/11/2024, 05/02/2025, 07/05/2025, 05/08/2025, 05/11/2025, 05/02/2026, 07/05/2026, 05/08/2026, 05/11/2026, 05/02/2027, 06/05/2027, 05/08/2027, 05/11/2027, 07/02/2028, 09/05/2028, 07/08/2028, 06/11/2028, 05/02/2029, 08/05/2029, 06/08/2029, 05/11/2029, 05/02/2030, 07/05/2030, 05/08/2030, 05/11/2030, 05/02/2031, 07/05/2031, 05/08/2031, 05/11/2031, 05/02/2032, 06/05/2032</t>
+          <t>05/08/2022, 05/08/2022, 07/08/2023, 05/08/2024, 05/08/2025, 05/08/2026, 05/08/2027</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Dates de remboursement</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>07/08/2023, 05/08/2024, 05/08/2025, 05/08/2026</t>
         </is>
       </c>
     </row>

</xml_diff>